<commit_message>
daily template update + waterfall tools and month retrieving + GOST fixes
</commit_message>
<xml_diff>
--- a/templates/tmp.xlsx
+++ b/templates/tmp.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -544,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -568,10 +568,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -589,13 +595,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -969,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,41 +994,41 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -1041,28 +1042,28 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="21.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1081,8 +1082,8 @@
       <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1114,101 +1115,101 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:13" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:13" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15" s="8" t="s">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -1233,7 +1234,7 @@
       <c r="F16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>30</v>
       </c>
       <c r="H16" s="9" t="s">
@@ -1244,17 +1245,17 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8" t="s">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
@@ -1275,7 +1276,7 @@
       <c r="F18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="9" t="s">
@@ -1286,17 +1287,17 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
@@ -1317,7 +1318,7 @@
       <c r="F20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>50</v>
       </c>
       <c r="H20" s="9" t="s">
@@ -1328,17 +1329,17 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21" s="8" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
@@ -1359,7 +1360,7 @@
       <c r="F22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="9" t="s">
         <v>60</v>
       </c>
       <c r="H22" s="9" t="s">
@@ -1370,17 +1371,17 @@
       </c>
     </row>
     <row r="23" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23" s="8" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -1401,7 +1402,7 @@
       <c r="F24" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>70</v>
       </c>
       <c r="H24" s="9" t="s">
@@ -1412,17 +1413,17 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25" s="8" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -1443,7 +1444,7 @@
       <c r="F26" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>80</v>
       </c>
       <c r="H26" s="9" t="s">
@@ -1454,17 +1455,17 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27" s="8" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -1485,7 +1486,7 @@
       <c r="F28" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>90</v>
       </c>
       <c r="H28" s="9" t="s">
@@ -1496,17 +1497,17 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29" s="8" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
     </row>
     <row r="30" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -1527,7 +1528,7 @@
       <c r="F30" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>100</v>
       </c>
       <c r="H30" s="9" t="s">
@@ -1538,17 +1539,17 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31" s="8" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -1569,7 +1570,7 @@
       <c r="F32" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="9" t="s">
         <v>110</v>
       </c>
       <c r="H32" s="9" t="s">
@@ -1580,13 +1581,17 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="8" t="s">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
@@ -1607,7 +1612,7 @@
       <c r="F34" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="9" t="s">
         <v>120</v>
       </c>
       <c r="H34" s="9" t="s">
@@ -1618,13 +1623,17 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="8" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
     </row>
     <row r="36" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
@@ -1645,7 +1654,7 @@
       <c r="F36" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="9" t="s">
         <v>130</v>
       </c>
       <c r="H36" s="9" t="s">
@@ -1656,13 +1665,17 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E37" s="8" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" s="6" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
@@ -1683,7 +1696,7 @@
       <c r="F38" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="9" t="s">
         <v>140</v>
       </c>
       <c r="H38" s="9" t="s">
@@ -1695,6 +1708,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
@@ -1703,14 +1724,6 @@
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="F12:H12"/>
   </mergeCells>
   <pageMargins left="0.98402777777777795" right="0.39374999999999999" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>